<commit_message>
Versión Python. Refactorización y nueva restricción de equilibrado de palets con restos.
</commit_message>
<xml_diff>
--- a/Analisis Resultados/Python/Análisis_PythonCBC_CubeMaster_Alimerka.xlsx
+++ b/Analisis Resultados/Python/Análisis_PythonCBC_CubeMaster_Alimerka.xlsx
@@ -21,14 +21,14 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId4"/>
-    <pivotCache cacheId="38" r:id="rId5"/>
+    <pivotCache cacheId="14" r:id="rId4"/>
+    <pivotCache cacheId="21" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="44">
   <si>
     <t>Load Summary</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>m</t>
-  </si>
-  <si>
-    <t>PALET-006(731-1984517-AL)</t>
   </si>
 </sst>
 </file>
@@ -661,13 +658,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -782,19 +781,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Federico Muñoz" refreshedDate="42511.514141898151" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="20">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Federico Muñoz" refreshedDate="42511.743682870372" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="20">
   <cacheSource type="worksheet">
     <worksheetSource ref="A4:H24" sheet="CBC"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Container" numFmtId="0">
-      <sharedItems count="6">
+      <sharedItems count="5">
         <s v="PALET-001(731-1984517-AL)"/>
         <s v="PALET-002(731-1984517-AL)"/>
         <s v="PALET-003(731-1984517-AL)"/>
         <s v="PALET-004(731-1984517-AL)"/>
         <s v="PALET-005(731-1984517-AL)"/>
-        <s v="PALET-006(731-1984517-AL)"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Loaded" numFmtId="0">
@@ -804,7 +802,7 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100" maxValue="100"/>
     </cacheField>
     <cacheField name="Area Effi." numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="16" maxValue="32"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="32" maxValue="32"/>
     </cacheField>
     <cacheField name="SKU" numFmtId="0">
       <sharedItems count="3">
@@ -1074,7 +1072,17 @@
     <x v="4"/>
     <n v="100"/>
     <n v="100"/>
-    <n v="16"/>
+    <n v="32"/>
+    <x v="2"/>
+    <n v="8"/>
+    <n v="1"/>
+    <n v="999999"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="100"/>
+    <n v="100"/>
+    <n v="32"/>
     <x v="0"/>
     <n v="8"/>
     <n v="2"/>
@@ -1084,27 +1092,17 @@
     <x v="4"/>
     <n v="100"/>
     <n v="100"/>
-    <n v="16"/>
+    <n v="32"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="4"/>
+    <n v="3"/>
     <n v="999999"/>
   </r>
   <r>
-    <x v="5"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="16"/>
-    <x v="2"/>
-    <n v="8"/>
-    <n v="1"/>
-    <n v="999999"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="16"/>
+    <x v="4"/>
+    <n v="100"/>
+    <n v="100"/>
+    <n v="32"/>
     <x v="2"/>
     <n v="8"/>
     <n v="4"/>
@@ -1114,7 +1112,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -1196,17 +1194,16 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="38" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="E3:G11" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="6">
+      <items count="5">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
-        <item x="5"/>
       </items>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -1253,8 +1250,7 @@
       <x v="4"/>
       <x/>
     </i>
-    <i>
-      <x v="5"/>
+    <i r="1">
       <x v="2"/>
     </i>
     <i t="grand">
@@ -1542,7 +1538,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G11" sqref="E1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1558,11 +1554,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G1">
-        <v>0.99</v>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6">
+        <v>0.65</v>
       </c>
       <c r="H1" t="s">
         <v>36</v>
@@ -1576,14 +1573,21 @@
       <c r="L1" s="5" t="s">
         <v>43</v>
       </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1595,13 +1599,13 @@
       <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1615,13 +1619,13 @@
       <c r="C5" s="2">
         <v>32</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="7">
         <v>32</v>
       </c>
     </row>
@@ -1635,13 +1639,13 @@
       <c r="C6" s="2">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="7">
         <v>32</v>
       </c>
     </row>
@@ -1655,13 +1659,13 @@
       <c r="C7" s="2">
         <v>32</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="7">
         <v>32</v>
       </c>
     </row>
@@ -1675,13 +1679,13 @@
       <c r="C8" s="2">
         <v>32</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="7">
         <v>32</v>
       </c>
     </row>
@@ -1695,13 +1699,13 @@
       <c r="C9" s="2">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="7">
         <v>16</v>
       </c>
     </row>
@@ -1715,13 +1719,13 @@
       <c r="C10" s="2">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="7">
         <v>16</v>
       </c>
     </row>
@@ -1732,10 +1736,11 @@
       <c r="C11" s="2">
         <v>160</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="2">
+      <c r="F11" s="6"/>
+      <c r="G11" s="7">
         <v>160</v>
       </c>
     </row>
@@ -2528,16 +2533,16 @@
         <v>100</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F21">
         <v>8</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>999999</v>
@@ -2554,7 +2559,7 @@
         <v>100</v>
       </c>
       <c r="D22">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
@@ -2563,7 +2568,7 @@
         <v>8</v>
       </c>
       <c r="G22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>999999</v>
@@ -2571,7 +2576,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -2580,16 +2585,16 @@
         <v>100</v>
       </c>
       <c r="D23">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F23">
         <v>8</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H23">
         <v>999999</v>
@@ -2597,7 +2602,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>100</v>
@@ -2606,7 +2611,7 @@
         <v>100</v>
       </c>
       <c r="D24">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
PLOS - Inclusión de restricción para no permitir más de dos columnas mixtas
</commit_message>
<xml_diff>
--- a/Analisis Resultados/Python/Análisis_PythonCBC_CubeMaster_Alimerka.xlsx
+++ b/Analisis Resultados/Python/Análisis_PythonCBC_CubeMaster_Alimerka.xlsx
@@ -19,10 +19,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CBC!$A$1:$E$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId4"/>
-    <pivotCache cacheId="21" r:id="rId5"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="18" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -658,7 +658,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -666,7 +666,6 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -763,7 +762,10 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Cargo/Layer" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="4"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="4" count="2">
+        <n v="4"/>
+        <n v="0"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Layer/Pallet" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="8"/>
@@ -781,7 +783,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Federico Muñoz" refreshedDate="42511.743682870372" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="20">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Federico Muñoz" refreshedDate="42570.755379282411" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="20">
   <cacheSource type="worksheet">
     <worksheetSource ref="A4:H24" sheet="CBC"/>
   </cacheSource>
@@ -796,13 +798,13 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Loaded" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100" maxValue="100"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="32" maxValue="32"/>
     </cacheField>
     <cacheField name="Vol. Effi." numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100" maxValue="100"/>
     </cacheField>
     <cacheField name="Area Effi." numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="32" maxValue="32"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100" maxValue="100"/>
     </cacheField>
     <cacheField name="SKU" numFmtId="0">
       <sharedItems count="3">
@@ -815,10 +817,15 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="8"/>
     </cacheField>
     <cacheField name="Column #" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="4">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Customer Product Code" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="999999" maxValue="999999"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="430082" maxValue="430135"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -839,7 +846,7 @@
     <x v="0"/>
     <n v="32"/>
     <s v="Alimerka"/>
-    <n v="4"/>
+    <x v="0"/>
     <n v="8"/>
     <n v="430082"/>
   </r>
@@ -851,7 +858,7 @@
     <x v="0"/>
     <n v="32"/>
     <s v="Alimerka"/>
-    <n v="4"/>
+    <x v="0"/>
     <n v="8"/>
     <n v="430082"/>
   </r>
@@ -863,7 +870,7 @@
     <x v="1"/>
     <n v="32"/>
     <s v="Alimerka"/>
-    <n v="4"/>
+    <x v="0"/>
     <n v="8"/>
     <n v="430117"/>
   </r>
@@ -875,7 +882,7 @@
     <x v="1"/>
     <n v="32"/>
     <s v="Alimerka"/>
-    <n v="4"/>
+    <x v="0"/>
     <n v="8"/>
     <n v="430117"/>
   </r>
@@ -887,7 +894,7 @@
     <x v="0"/>
     <n v="16"/>
     <s v="Alimerka"/>
-    <n v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <n v="430082"/>
   </r>
@@ -899,7 +906,7 @@
     <x v="2"/>
     <n v="16"/>
     <s v="Alimerka"/>
-    <n v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <n v="430135"/>
   </r>
@@ -910,209 +917,209 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
   <r>
     <x v="0"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="1"/>
-    <n v="999999"/>
+    <x v="0"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="2"/>
-    <n v="999999"/>
+    <x v="1"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="3"/>
-    <n v="999999"/>
+    <x v="2"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="4"/>
-    <n v="999999"/>
+    <x v="3"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="1"/>
-    <n v="999999"/>
+    <x v="0"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="2"/>
-    <n v="999999"/>
+    <x v="1"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="3"/>
-    <n v="999999"/>
+    <x v="2"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="4"/>
-    <n v="999999"/>
+    <x v="3"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="2"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="1"/>
     <n v="8"/>
-    <n v="1"/>
-    <n v="999999"/>
+    <x v="0"/>
+    <n v="430117"/>
   </r>
   <r>
     <x v="2"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="1"/>
     <n v="8"/>
-    <n v="2"/>
-    <n v="999999"/>
+    <x v="1"/>
+    <n v="430117"/>
   </r>
   <r>
     <x v="2"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="1"/>
     <n v="8"/>
-    <n v="3"/>
-    <n v="999999"/>
+    <x v="2"/>
+    <n v="430117"/>
   </r>
   <r>
     <x v="2"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="1"/>
     <n v="8"/>
-    <n v="4"/>
-    <n v="999999"/>
+    <x v="3"/>
+    <n v="430117"/>
   </r>
   <r>
     <x v="3"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="1"/>
     <n v="8"/>
-    <n v="1"/>
-    <n v="999999"/>
+    <x v="0"/>
+    <n v="430117"/>
   </r>
   <r>
     <x v="3"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="1"/>
     <n v="8"/>
-    <n v="2"/>
-    <n v="999999"/>
+    <x v="1"/>
+    <n v="430117"/>
   </r>
   <r>
     <x v="3"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="1"/>
     <n v="8"/>
-    <n v="3"/>
-    <n v="999999"/>
+    <x v="2"/>
+    <n v="430117"/>
   </r>
   <r>
     <x v="3"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="1"/>
     <n v="8"/>
-    <n v="4"/>
-    <n v="999999"/>
+    <x v="3"/>
+    <n v="430117"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
-    <x v="2"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
+    <x v="0"/>
     <n v="8"/>
-    <n v="1"/>
-    <n v="999999"/>
+    <x v="0"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="0"/>
     <n v="8"/>
-    <n v="2"/>
-    <n v="999999"/>
+    <x v="1"/>
+    <n v="430082"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
-    <x v="0"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
+    <x v="2"/>
     <n v="8"/>
-    <n v="3"/>
-    <n v="999999"/>
+    <x v="2"/>
+    <n v="430135"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="100"/>
-    <n v="100"/>
-    <n v="32"/>
+    <n v="32"/>
+    <n v="100"/>
+    <n v="100"/>
     <x v="2"/>
     <n v="8"/>
-    <n v="4"/>
-    <n v="999999"/>
+    <x v="3"/>
+    <n v="430135"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -1142,7 +1149,13 @@
     </pivotField>
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
   </pivotFields>
@@ -1194,7 +1207,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable8" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="E3:G11" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -1222,7 +1235,14 @@
       </items>
     </pivotField>
     <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
@@ -1348,6 +1368,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1383,6 +1420,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1538,16 +1592,17 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="E1:G11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.6328125" customWidth="1"/>
-    <col min="3" max="4" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.08984375" customWidth="1"/>
+    <col min="4" max="4" width="5.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6328125" customWidth="1"/>
+    <col min="6" max="6" width="24.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="5.08984375" customWidth="1"/>
     <col min="9" max="9" width="24.7265625" customWidth="1"/>
     <col min="10" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
@@ -1559,7 +1614,7 @@
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6">
-        <v>0.65</v>
+        <v>0.35</v>
       </c>
       <c r="H1" t="s">
         <v>36</v>
@@ -1583,11 +1638,9 @@
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1599,13 +1652,13 @@
       <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1619,13 +1672,13 @@
       <c r="C5" s="2">
         <v>32</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="2">
         <v>32</v>
       </c>
     </row>
@@ -1639,13 +1692,13 @@
       <c r="C6" s="2">
         <v>32</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="2">
         <v>32</v>
       </c>
     </row>
@@ -1659,13 +1712,13 @@
       <c r="C7" s="2">
         <v>32</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="2">
         <v>32</v>
       </c>
     </row>
@@ -1679,13 +1732,13 @@
       <c r="C8" s="2">
         <v>32</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="2">
         <v>32</v>
       </c>
     </row>
@@ -1699,13 +1752,13 @@
       <c r="C9" s="2">
         <v>16</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="2">
         <v>16</v>
       </c>
     </row>
@@ -1719,13 +1772,13 @@
       <c r="C10" s="2">
         <v>16</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="2">
         <v>16</v>
       </c>
     </row>
@@ -1736,11 +1789,10 @@
       <c r="C11" s="2">
         <v>160</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7">
+      <c r="G11" s="2">
         <v>160</v>
       </c>
     </row>
@@ -2053,12 +2105,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="24.26953125" bestFit="1" customWidth="1"/>
@@ -2111,13 +2164,13 @@
         <v>23</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
       <c r="D5">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -2129,7 +2182,7 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -2137,13 +2190,13 @@
         <v>23</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -2155,7 +2208,7 @@
         <v>2</v>
       </c>
       <c r="H6">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -2163,13 +2216,13 @@
         <v>23</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="D7">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -2181,7 +2234,7 @@
         <v>3</v>
       </c>
       <c r="H7">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -2189,13 +2242,13 @@
         <v>23</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>100</v>
       </c>
       <c r="D8">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
@@ -2207,7 +2260,7 @@
         <v>4</v>
       </c>
       <c r="H8">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -2215,13 +2268,13 @@
         <v>25</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
       <c r="D9">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -2233,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -2241,13 +2294,13 @@
         <v>25</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>100</v>
       </c>
       <c r="D10">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -2259,7 +2312,7 @@
         <v>2</v>
       </c>
       <c r="H10">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -2267,13 +2320,13 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>100</v>
       </c>
       <c r="D11">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
@@ -2285,7 +2338,7 @@
         <v>3</v>
       </c>
       <c r="H11">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -2293,13 +2346,13 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>100</v>
       </c>
       <c r="D12">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -2311,7 +2364,7 @@
         <v>4</v>
       </c>
       <c r="H12">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -2319,13 +2372,13 @@
         <v>26</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>100</v>
       </c>
       <c r="D13">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
@@ -2337,7 +2390,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>999999</v>
+        <v>430117</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -2345,13 +2398,13 @@
         <v>26</v>
       </c>
       <c r="B14">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>100</v>
       </c>
       <c r="D14">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
@@ -2363,7 +2416,7 @@
         <v>2</v>
       </c>
       <c r="H14">
-        <v>999999</v>
+        <v>430117</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -2371,13 +2424,13 @@
         <v>26</v>
       </c>
       <c r="B15">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>100</v>
       </c>
       <c r="D15">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E15" t="s">
         <v>27</v>
@@ -2389,7 +2442,7 @@
         <v>3</v>
       </c>
       <c r="H15">
-        <v>999999</v>
+        <v>430117</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -2397,13 +2450,13 @@
         <v>26</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>100</v>
       </c>
       <c r="D16">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
         <v>27</v>
@@ -2415,7 +2468,7 @@
         <v>4</v>
       </c>
       <c r="H16">
-        <v>999999</v>
+        <v>430117</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -2423,13 +2476,13 @@
         <v>28</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>100</v>
       </c>
       <c r="D17">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E17" t="s">
         <v>27</v>
@@ -2441,7 +2494,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>999999</v>
+        <v>430117</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -2449,13 +2502,13 @@
         <v>28</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>100</v>
       </c>
       <c r="D18">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
         <v>27</v>
@@ -2467,7 +2520,7 @@
         <v>2</v>
       </c>
       <c r="H18">
-        <v>999999</v>
+        <v>430117</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -2475,13 +2528,13 @@
         <v>28</v>
       </c>
       <c r="B19">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>100</v>
       </c>
       <c r="D19">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
         <v>27</v>
@@ -2493,7 +2546,7 @@
         <v>3</v>
       </c>
       <c r="H19">
-        <v>999999</v>
+        <v>430117</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -2501,13 +2554,13 @@
         <v>28</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>100</v>
       </c>
       <c r="D20">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
@@ -2519,7 +2572,7 @@
         <v>4</v>
       </c>
       <c r="H20">
-        <v>999999</v>
+        <v>430117</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -2527,16 +2580,16 @@
         <v>29</v>
       </c>
       <c r="B21">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>100</v>
       </c>
       <c r="D21">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -2545,7 +2598,7 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -2553,13 +2606,13 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>100</v>
       </c>
       <c r="D22">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
@@ -2571,7 +2624,7 @@
         <v>2</v>
       </c>
       <c r="H22">
-        <v>999999</v>
+        <v>430082</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -2579,16 +2632,16 @@
         <v>29</v>
       </c>
       <c r="B23">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>100</v>
       </c>
       <c r="D23">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F23">
         <v>8</v>
@@ -2597,7 +2650,7 @@
         <v>3</v>
       </c>
       <c r="H23">
-        <v>999999</v>
+        <v>430135</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -2605,13 +2658,13 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>100</v>
       </c>
       <c r="D24">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
         <v>30</v>
@@ -2623,7 +2676,7 @@
         <v>4</v>
       </c>
       <c r="H24">
-        <v>999999</v>
+        <v>430135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>